<commit_message>
Correct error in LIPS trial
had the LDL for PBO and F transposed
</commit_message>
<xml_diff>
--- a/secprevstatin_yrly.xlsx
+++ b/secprevstatin_yrly.xlsx
@@ -5,21 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\HSLLC\La_Rossa_line\rawdat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\LDLCVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10668"/>
   </bookViews>
   <sheets>
     <sheet name="secprevstatin_yrly" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -38,13 +33,22 @@
     <t>LDL</t>
   </si>
   <si>
+    <t>cases</t>
+  </si>
+  <si>
+    <t>eventrate</t>
+  </si>
+  <si>
+    <t>lastrand</t>
+  </si>
+  <si>
     <t>f_meanure</t>
   </si>
   <si>
     <t>followup</t>
   </si>
   <si>
-    <t>eventrate</t>
+    <t>outcome</t>
   </si>
   <si>
     <t>TNT</t>
@@ -53,25 +57,25 @@
     <t>A80</t>
   </si>
   <si>
-    <t>cases</t>
-  </si>
-  <si>
-    <t>lastrand</t>
-  </si>
-  <si>
     <t>median</t>
   </si>
   <si>
+    <t>CVDeath, nfMI</t>
+  </si>
+  <si>
     <t>A10</t>
   </si>
   <si>
     <t>HPS</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>mean</t>
   </si>
   <si>
-    <t>S</t>
+    <t>CorDeath, nfMI</t>
   </si>
   <si>
     <t>PBO</t>
@@ -83,74 +87,65 @@
     <t>P</t>
   </si>
   <si>
+    <t>CHDDeath, nfMI</t>
+  </si>
+  <si>
     <t>LIPID</t>
   </si>
   <si>
     <t>4S</t>
   </si>
   <si>
+    <t>CorDeath, nfMI, resCA</t>
+  </si>
+  <si>
+    <t>IDEAL</t>
+  </si>
+  <si>
     <t>S20</t>
   </si>
   <si>
-    <t>IDEAL</t>
+    <t>CHDDeath, nfMI, resCA</t>
+  </si>
+  <si>
+    <t>LIPS</t>
+  </si>
+  <si>
+    <t>mean/med</t>
+  </si>
+  <si>
+    <t>CorDeath/nfMI</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>GREACE</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AVERT</t>
+  </si>
+  <si>
+    <t>CarDeath/nfMI</t>
   </si>
   <si>
     <t>PROVEIT</t>
   </si>
   <si>
     <t>P40</t>
-  </si>
-  <si>
-    <t>outcome</t>
-  </si>
-  <si>
-    <t>CVDeath, nfMI</t>
-  </si>
-  <si>
-    <t>CorDeath, nfMI</t>
-  </si>
-  <si>
-    <t>CHDDeath, nfMI</t>
-  </si>
-  <si>
-    <t>CorDeath, nfMI, resCA</t>
-  </si>
-  <si>
-    <t>CHDDeath, nfMI, resCA</t>
-  </si>
-  <si>
-    <t>LIPS</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>GREACE</t>
-  </si>
-  <si>
-    <t>UC</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>AVERT</t>
-  </si>
-  <si>
-    <t>mean/med</t>
-  </si>
-  <si>
-    <t>CorDeath/nfMI</t>
-  </si>
-  <si>
-    <t>CarDeath/nfMI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,16 +153,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -175,16 +470,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -464,17 +947,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.21875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -490,30 +965,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>4995</v>
@@ -531,181 +1006,181 @@
         <v>199912</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>4.9000000000000004</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>5006</v>
+      </c>
+      <c r="D3">
+        <v>101</v>
+      </c>
+      <c r="E3">
+        <v>418</v>
+      </c>
+      <c r="F3">
+        <v>1.8</v>
+      </c>
+      <c r="G3">
+        <v>199912</v>
+      </c>
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
-        <v>5006</v>
-      </c>
-      <c r="D3" s="1">
-        <v>101</v>
-      </c>
-      <c r="E3" s="1">
-        <v>418</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="G3" s="1">
-        <v>199912</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="I3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
         <v>10269</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>88.941000000000003</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>898</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>1.75</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
         <v>199705</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4">
         <v>5</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
         <v>10267</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>127.611</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>1212</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>2.36</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5">
         <v>199705</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5">
         <v>5</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="J5" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
         <v>2081</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>96.674999999999997</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>212</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>2.04</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6">
         <v>199112</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
         <v>2078</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>134.26</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>274</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>2.64</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <v>199112</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>28</v>
+      <c r="J7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>4512</v>
@@ -723,21 +1198,21 @@
         <v>199212</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I8">
         <v>6.1</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
       </c>
       <c r="C9">
         <v>4502</v>
@@ -755,21 +1230,21 @@
         <v>199212</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I9">
         <v>6.1</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>2221</v>
@@ -787,21 +1262,21 @@
         <v>198908</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I10">
         <v>5.4</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>2223</v>
@@ -819,21 +1294,21 @@
         <v>198908</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I11">
         <v>5.4</v>
       </c>
       <c r="J11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>4449</v>
@@ -851,21 +1326,21 @@
         <v>200103</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12">
         <v>4.8</v>
       </c>
       <c r="J12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>4439</v>
@@ -883,27 +1358,27 @@
         <v>200103</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I13">
         <v>4.8</v>
       </c>
       <c r="J13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>833</v>
       </c>
       <c r="D14">
-        <v>95.63</v>
+        <v>146.52000000000001</v>
       </c>
       <c r="E14">
         <v>60</v>
@@ -915,18 +1390,18 @@
         <v>199810</v>
       </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I14">
         <v>3.9</v>
       </c>
       <c r="J14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
@@ -935,7 +1410,7 @@
         <v>844</v>
       </c>
       <c r="D15">
-        <v>146.52000000000001</v>
+        <v>95.63</v>
       </c>
       <c r="E15">
         <v>42</v>
@@ -947,13 +1422,13 @@
         <v>199810</v>
       </c>
       <c r="H15" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I15">
         <v>3.9</v>
       </c>
       <c r="J15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -979,13 +1454,13 @@
         <v>200012</v>
       </c>
       <c r="H16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I16">
         <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1011,13 +1486,13 @@
         <v>200012</v>
       </c>
       <c r="H17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I17">
         <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1043,21 +1518,21 @@
         <v>199612</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I18">
         <v>1.5</v>
       </c>
       <c r="J18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <v>2063</v>
@@ -1072,21 +1547,21 @@
         <v>200112</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I19">
         <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>2099</v>
@@ -1101,16 +1576,17 @@
         <v>200112</v>
       </c>
       <c r="H20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I20">
         <v>2</v>
       </c>
       <c r="J20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>